<commit_message>
changes in online speakers
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="13850" windowHeight="7130"/>
+    <workbookView activeTab="1" windowWidth="13850" windowHeight="7130"/>
   </bookViews>
   <sheets>
     <sheet name="With annotations" sheetId="1" r:id="rId1"/>
@@ -36,72 +36,14 @@
     <author>Tarmo Uustalu</author>
   </authors>
   <commentList>
-    <comment ref="Q19" authorId="0">
-      <text>
-        <t>Olarte, Waddington, Barroso-Nascimento, Studer
-</t>
-      </text>
-    </comment>
-    <comment ref="R19" authorId="0">
-      <text>
-        <t>Stark, Yulu Pan
-</t>
-      </text>
-    </comment>
-    <comment ref="V22" authorId="0">
-      <text>
-        <t>Bjarki</t>
-      </text>
-    </comment>
-    <comment ref="U22" authorId="0">
-      <text>
-        <t>Bjarki	
-</t>
-      </text>
-    </comment>
-    <comment ref="S19" authorId="0">
-      <text>
-        <t>Hähnle, Ramanayake, Jalali
-</t>
-      </text>
-    </comment>
-    <comment ref="P19" authorId="0">
-      <text>
-        <t>Jalali
-</t>
-      </text>
-    </comment>
-    <comment ref="P22" authorId="0">
-      <text>
-        <t>Antonis, Vasiliki
-</t>
-      </text>
-    </comment>
-    <comment ref="U19" authorId="0">
-      <text>
-        <t>Yoshida, H Barbosa
-</t>
-      </text>
-    </comment>
-    <comment ref="T19" authorId="0">
-      <text>
-        <t>Yoshida</t>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <t>Motalebi changed from Tableaux Saver Early to Tbl+Fro online presenter</t>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="C5" authorId="0">
       <text>
-        <t>Changed Affeldt changed from ITP Saver Late to ITP Full Early
-</t>
-      </text>
-    </comment>
-    <comment ref="I5" authorId="0">
-      <text>
-        <t>Changed Affeldt changed from ITP Saver Late to ITP Full Early
+        <t>Sehun Kim cancelled (fully)
 </t>
       </text>
     </comment>
@@ -113,15 +55,73 @@
 </t>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="I5" authorId="0">
       <text>
-        <t>Sehun Kim cancelled (fully)
+        <t>Changed Affeldt changed from ITP Saver Late to ITP Full Early
 </t>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="B5" authorId="0">
+      <text>
+        <t>Changed Affeldt changed from ITP Saver Late to ITP Full Early
+</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0">
       <text>
         <t>Motalebi changed from Tableaux Saver Early to Tbl+Fro online presenter</t>
+      </text>
+    </comment>
+    <comment ref="T19" authorId="0">
+      <text>
+        <t>Yoshida</t>
+      </text>
+    </comment>
+    <comment ref="U19" authorId="0">
+      <text>
+        <t>Yoshida, H Barbosa
+</t>
+      </text>
+    </comment>
+    <comment ref="P22" authorId="0">
+      <text>
+        <t>Antonis, Vasiliki
+</t>
+      </text>
+    </comment>
+    <comment ref="P19" authorId="0">
+      <text>
+        <t>Jalali
+</t>
+      </text>
+    </comment>
+    <comment ref="S19" authorId="0">
+      <text>
+        <t>Hähnle, Ramanayake, Jalali
+</t>
+      </text>
+    </comment>
+    <comment ref="U22" authorId="0">
+      <text>
+        <t>Bjarki	
+</t>
+      </text>
+    </comment>
+    <comment ref="V22" authorId="0">
+      <text>
+        <t>Bjarki</t>
+      </text>
+    </comment>
+    <comment ref="R19" authorId="0">
+      <text>
+        <t>Stark, Yulu Pan
+</t>
+      </text>
+    </comment>
+    <comment ref="Q19" authorId="0">
+      <text>
+        <t>Olarte, Waddington, Barroso-Nascimento, Studer
+</t>
       </text>
     </comment>
   </commentList>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="145" count="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144" count="144">
   <si>
     <t>Sat 27 Sept</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>Serdar Erbatur, Andrew M. Marshall, Paliath Narendran and Christophe Ringeissen. Graph Embedded Rewrite Systems: Combination and Undecidability Results</t>
-  </si>
-  <si>
-    <t>Ringeissen</t>
   </si>
   <si>
     <t>Anshula Gandhi, Anand Rao Tadipatri, Timothy Gowers. Automatically Generalizing Proofs and Statements</t>
@@ -1029,7 +1026,7 @@
   </sheetPr>
   <dimension ref="A1:IV65538"/>
   <sheetViews>
-    <sheetView topLeftCell="C59" workbookViewId="0" tabSelected="1">
+    <sheetView topLeftCell="C59" workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
@@ -3627,8 +3624,10 @@
       <c r="E78" s="4">
         <v>1</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>74</v>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>Ringeissen</t>
+        </is>
       </c>
     </row>
     <row r="79" spans="1:256">
@@ -3660,7 +3659,7 @@
     <row r="81" spans="1:256" ht="26.25">
       <c r="A81" s="4"/>
       <c r="B81" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C81" s="12" t="inlineStr">
         <is>
@@ -3668,7 +3667,7 @@
         </is>
       </c>
       <c r="D81" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E81" s="4" t="inlineStr">
         <is>
@@ -3680,7 +3679,7 @@
     <row r="82" spans="1:256" ht="13.5">
       <c r="A82" s="4"/>
       <c r="B82" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C82" s="12"/>
       <c r="D82" s="25"/>
@@ -3690,7 +3689,7 @@
     <row r="83" spans="1:256" ht="26.25">
       <c r="A83" s="4"/>
       <c r="B83" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83" s="12" t="inlineStr">
         <is>
@@ -3698,7 +3697,7 @@
         </is>
       </c>
       <c r="D83" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E83" s="4">
         <v>23</v>
@@ -3742,7 +3741,7 @@
       </c>
       <c r="C86" s="27"/>
       <c r="D86" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E86" s="4">
         <v>4</v>
@@ -3756,11 +3755,11 @@
     <row r="87" spans="1:256" ht="26.25">
       <c r="A87" s="4"/>
       <c r="B87" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87" s="27"/>
       <c r="D87" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E87" s="4">
         <v>16</v>
@@ -3776,7 +3775,7 @@
       <c r="B88" s="26"/>
       <c r="C88" s="19"/>
       <c r="D88" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E88" s="4">
         <v>26</v>
@@ -3797,7 +3796,7 @@
     </row>
     <row r="90" spans="1:256" ht="13.5">
       <c r="A90" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>18</v>
@@ -4088,7 +4087,7 @@
     <row r="93" spans="1:256" ht="39">
       <c r="A93" s="4"/>
       <c r="B93" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C93" s="12" t="inlineStr">
         <is>
@@ -4096,7 +4095,7 @@
         </is>
       </c>
       <c r="D93" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E93" s="4">
         <v>7</v>
@@ -4110,7 +4109,7 @@
     <row r="94" spans="1:256" ht="26.25">
       <c r="A94" s="4"/>
       <c r="B94" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C94" s="12" t="inlineStr">
         <is>
@@ -4118,7 +4117,7 @@
         </is>
       </c>
       <c r="D94" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E94" s="4">
         <v>9</v>
@@ -4132,7 +4131,7 @@
     <row r="95" spans="1:256" ht="26.25">
       <c r="A95" s="4"/>
       <c r="B95" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C95" s="12" t="inlineStr">
         <is>
@@ -4140,7 +4139,7 @@
         </is>
       </c>
       <c r="D95" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E95" s="4">
         <v>2</v>
@@ -4180,7 +4179,7 @@
     <row r="98" spans="1:256" ht="26.25">
       <c r="A98" s="4"/>
       <c r="B98" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C98" s="12" t="inlineStr">
         <is>
@@ -4188,7 +4187,7 @@
         </is>
       </c>
       <c r="D98" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E98" s="4">
         <v>8</v>
@@ -4202,7 +4201,7 @@
     <row r="99" spans="1:256" ht="26.25">
       <c r="A99" s="4"/>
       <c r="B99" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C99" s="12" t="inlineStr">
         <is>
@@ -4226,7 +4225,7 @@
     <row r="100" spans="1:256" ht="26.25">
       <c r="A100" s="4"/>
       <c r="B100" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" s="28" t="inlineStr">
         <is>
@@ -4234,7 +4233,7 @@
         </is>
       </c>
       <c r="D100" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E100" s="4">
         <v>28</v>
@@ -4274,7 +4273,7 @@
     <row r="103" spans="1:256" ht="26.25">
       <c r="A103" s="4"/>
       <c r="B103" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C103" s="12" t="inlineStr">
         <is>
@@ -4282,7 +4281,7 @@
         </is>
       </c>
       <c r="D103" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E103" s="4">
         <v>18</v>
@@ -4296,7 +4295,7 @@
     <row r="104" spans="1:256" ht="26.25">
       <c r="A104" s="4"/>
       <c r="B104" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C104" s="12" t="inlineStr">
         <is>
@@ -4320,7 +4319,7 @@
     <row r="105" spans="1:256" ht="13.5">
       <c r="A105" s="4"/>
       <c r="B105" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105" s="12" t="inlineStr">
         <is>
@@ -4358,7 +4357,7 @@
     <row r="108" spans="1:256" ht="26.25">
       <c r="A108" s="4"/>
       <c r="B108" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C108" s="12" t="inlineStr">
         <is>
@@ -4372,7 +4371,7 @@
     <row r="109" spans="1:256" ht="26.25">
       <c r="A109" s="4"/>
       <c r="B109" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C109" s="12" t="inlineStr">
         <is>
@@ -4386,7 +4385,7 @@
     <row r="110" spans="1:256" ht="39">
       <c r="A110" s="4"/>
       <c r="B110" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C110" s="12" t="inlineStr">
         <is>
@@ -4423,10 +4422,10 @@
     </row>
     <row r="113" spans="1:256" ht="13.5">
       <c r="A113" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B113" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -5664,8 +5663,8 @@
   </sheetPr>
   <dimension ref="A1:XFD65543"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A109" workbookViewId="0" tabSelected="1">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6453,7 +6452,7 @@
         </is>
       </c>
       <c r="C5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -6709,7 +6708,7 @@
     </row>
     <row r="7" spans="1:16384" customHeight="1" ht="15.75">
       <c r="A7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="30" t="inlineStr">
         <is>
@@ -6764,7 +6763,7 @@
     </row>
     <row r="12" spans="1:16384" customHeight="1" ht="15">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="30" t="inlineStr">
         <is>
@@ -6820,7 +6819,7 @@
     </row>
     <row r="17" spans="1:16384" customHeight="1" ht="14.25">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="30" t="inlineStr">
         <is>
@@ -6873,7 +6872,7 @@
     </row>
     <row r="22" spans="1:16384" ht="13.5">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="30" t="inlineStr">
         <is>
@@ -6938,10 +6937,10 @@
         <v>17</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -7197,7 +7196,7 @@
     </row>
     <row r="30" spans="1:16384" ht="13.5">
       <c r="A30" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="32" t="inlineStr">
         <is>
@@ -7215,8 +7214,10 @@
       <c r="B31" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>20</v>
+      <c r="C31" s="9" t="inlineStr">
+        <is>
+          <t>Raheleh Jalali. Skolemization Beyond Intuitionistic Logic: The Role of Quantifier Shifts [online]</t>
+        </is>
       </c>
     </row>
     <row r="32" spans="1:16384" ht="26.25">
@@ -7242,7 +7243,7 @@
     </row>
     <row r="35" spans="1:16384" ht="13.5">
       <c r="A35" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" s="32" t="inlineStr">
         <is>
@@ -7662,7 +7663,7 @@
     </row>
     <row r="53" spans="1:16384" ht="13.5">
       <c r="A53" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" s="32" t="inlineStr">
         <is>
@@ -7832,7 +7833,7 @@
         <v>61</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C71" s="5" t="inlineStr">
         <is>
@@ -8093,7 +8094,7 @@
     </row>
     <row r="73" spans="1:16384" ht="13.5">
       <c r="A73" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B73" s="32" t="inlineStr">
         <is>
@@ -8112,7 +8113,7 @@
         <v>63</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D74" s="0"/>
     </row>
@@ -8139,7 +8140,7 @@
     </row>
     <row r="78" spans="1:16384" ht="13.5">
       <c r="A78" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" s="7" t="inlineStr">
         <is>
@@ -8187,7 +8188,7 @@
     <row r="83" spans="1:16384" ht="13.5">
       <c r="A83" s="4"/>
       <c r="B83" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C83" s="4"/>
     </row>
@@ -8211,26 +8212,26 @@
     <row r="85" spans="1:16384" ht="26.25">
       <c r="A85" s="4"/>
       <c r="B85" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:16384" customHeight="1" ht="27">
       <c r="A86" s="4"/>
       <c r="B86" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C86" s="17"/>
     </row>
     <row r="87" spans="1:16384" ht="26.25">
       <c r="A87" s="4"/>
       <c r="B87" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C87" s="35" t="s">
         <v>78</v>
-      </c>
-      <c r="C87" s="35" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:16384">
@@ -8261,13 +8262,13 @@
         <v>37</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:16384" ht="26.25">
       <c r="A91" s="4"/>
       <c r="B91" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C91" s="35" t="s">
         <v>64</v>
@@ -8278,7 +8279,7 @@
       <c r="A92" s="4"/>
       <c r="B92" s="23"/>
       <c r="C92" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:16384">
@@ -8288,10 +8289,10 @@
     </row>
     <row r="94" spans="1:16384" ht="13.5">
       <c r="A94" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C94" s="5" t="inlineStr">
         <is>
@@ -8552,7 +8553,7 @@
     </row>
     <row r="96" spans="1:16384" ht="13.5">
       <c r="A96" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" s="7" t="inlineStr">
         <is>
@@ -8568,28 +8569,28 @@
     <row r="97" spans="1:16384" ht="39">
       <c r="A97" s="4"/>
       <c r="B97" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C97" s="35" t="s">
         <v>85</v>
-      </c>
-      <c r="C97" s="35" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:16384" ht="26.25">
       <c r="A98" s="4"/>
       <c r="B98" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C98" s="35" t="s">
         <v>87</v>
-      </c>
-      <c r="C98" s="35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:16384" ht="26.25">
       <c r="A99" s="4"/>
       <c r="B99" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" s="35" t="s">
         <v>89</v>
-      </c>
-      <c r="C99" s="35" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:16384">
@@ -8599,7 +8600,7 @@
     </row>
     <row r="101" spans="1:16384" ht="13.5">
       <c r="A101" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B101" s="7" t="inlineStr">
         <is>
@@ -8615,16 +8616,16 @@
     <row r="102" spans="1:16384" ht="26.25">
       <c r="A102" s="4"/>
       <c r="B102" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C102" s="35" t="s">
         <v>91</v>
-      </c>
-      <c r="C102" s="35" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="103" spans="1:16384" ht="26.25">
       <c r="A103" s="4"/>
       <c r="B103" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C103" s="35" t="inlineStr">
         <is>
@@ -8635,10 +8636,10 @@
     <row r="104" spans="1:16384" ht="26.25">
       <c r="A104" s="4"/>
       <c r="B104" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C104" s="35" t="s">
         <v>94</v>
-      </c>
-      <c r="C104" s="35" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:16384">
@@ -8648,7 +8649,7 @@
     </row>
     <row r="106" spans="1:16384" ht="13.5">
       <c r="A106" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" s="7" t="inlineStr">
         <is>
@@ -8664,16 +8665,16 @@
     <row r="107" spans="1:16384" ht="26.25">
       <c r="A107" s="4"/>
       <c r="B107" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C107" s="35" t="s">
         <v>96</v>
-      </c>
-      <c r="C107" s="35" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="108" spans="1:16384" ht="26.25">
       <c r="A108" s="4"/>
       <c r="B108" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C108" s="35" t="inlineStr">
         <is>
@@ -8684,7 +8685,7 @@
     <row r="109" spans="1:16384" ht="13.5">
       <c r="A109" s="4"/>
       <c r="B109" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C109" s="17" t="s">
         <v>37</v>
@@ -8711,21 +8712,21 @@
     <row r="112" spans="1:16384" ht="26.25">
       <c r="A112" s="4"/>
       <c r="B112" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C112" s="4"/>
     </row>
     <row r="113" spans="1:16384" ht="26.25">
       <c r="A113" s="4"/>
       <c r="B113" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:16384" ht="39">
       <c r="A114" s="4"/>
       <c r="B114" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C114" s="4"/>
     </row>
@@ -8745,7 +8746,7 @@
     </row>
     <row r="117" spans="1:16384" ht="13.5">
       <c r="A117" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B117" s="5" t="inlineStr">
         <is>
@@ -9007,7 +9008,7 @@
     </row>
     <row r="119" spans="1:16384" ht="13.5">
       <c r="A119" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B119" s="30" t="inlineStr">
         <is>
@@ -9046,7 +9047,7 @@
     </row>
     <row r="124" spans="1:16384" ht="13.5">
       <c r="A124" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B124" s="30" t="inlineStr">
         <is>
@@ -9059,7 +9060,7 @@
       <c r="A125" s="4"/>
       <c r="B125" s="30" t="inlineStr">
         <is>
-          <t>Mauricio Barba da Costa. Automatic Geometry Theorem Proving Using Polynomial Elaboration (20 mins) [online]</t>
+          <t>Mauricio Barba da Costa. Automatic Geometry Theorem Proving Using Polynomial Elaboration (20 mins)</t>
         </is>
       </c>
       <c r="C125" s="4"/>
@@ -9068,7 +9069,7 @@
       <c r="A126" s="4"/>
       <c r="B126" s="30" t="inlineStr">
         <is>
-          <t>Moritz Firsching. The Formal Conjectures Repo (20 mins)</t>
+          <t>Moritz Firsching. The Formal Conjectures Repo (20 mins) [online]</t>
         </is>
       </c>
       <c r="C126" s="4"/>
@@ -9098,7 +9099,7 @@
     </row>
     <row r="130" spans="1:16384" ht="13.5">
       <c r="A130" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B130" s="30" t="inlineStr">
         <is>
@@ -9133,7 +9134,7 @@
     </row>
     <row r="135" spans="1:16384" ht="13.5">
       <c r="A135" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B135" s="30" t="inlineStr">
         <is>
@@ -26359,7 +26360,7 @@
   <sheetData>
     <row r="1" spans="1:251" customHeight="1" ht="15.75">
       <c r="A1" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -26867,10 +26868,10 @@
         </is>
       </c>
       <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -26878,10 +26879,10 @@
         </is>
       </c>
       <c r="F3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
         <v>113</v>
-      </c>
-      <c r="G3" t="s">
-        <v>114</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -27636,25 +27637,25 @@
     </row>
     <row r="7" spans="1:251" ht="13.5">
       <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
       </c>
       <c r="C7">
         <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
         <v>117</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
       </c>
       <c r="F7">
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:251" ht="13.5"/>
@@ -27921,25 +27922,25 @@
     <row r="11" spans="1:251" ht="12.75"/>
     <row r="12" spans="1:251" ht="13.5">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12">
         <v>74</v>
       </c>
       <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" t="s">
         <v>117</v>
-      </c>
-      <c r="E12" t="s">
-        <v>118</v>
       </c>
       <c r="F12">
         <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:251" ht="13.5"/>
@@ -28206,44 +28207,44 @@
     <row r="16" spans="1:251" ht="12.75"/>
     <row r="17" spans="1:251" ht="13.5">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17">
         <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" s="41">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:251" ht="13.5">
       <c r="G18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:251" ht="13.5">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20">
         <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -28254,7 +28255,7 @@
         <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -28264,7 +28265,7 @@
     </row>
     <row r="21" spans="1:251" ht="13.5">
       <c r="G21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -28541,25 +28542,25 @@
     <row r="24" spans="1:251" ht="12.75"/>
     <row r="25" spans="1:251" ht="13.5">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>75</v>
       </c>
       <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
         <v>129</v>
-      </c>
-      <c r="E25" t="s">
-        <v>130</v>
       </c>
       <c r="F25">
         <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -28597,25 +28598,25 @@
     </row>
     <row r="32" spans="1:251" ht="13.5">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32">
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F32">
         <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -28633,7 +28634,7 @@
     <row r="35" spans="1:251" ht="12.75"/>
     <row r="36" spans="1:251" ht="13.5">
       <c r="A36" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>18</v>
@@ -28893,62 +28894,62 @@
     <row r="37" spans="1:251" ht="12.75"/>
     <row r="38" spans="1:251" ht="13.5">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38">
         <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F38">
         <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:251" ht="13.5">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41">
         <v>74</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F41">
         <v>31</v>
       </c>
       <c r="G41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:251" ht="13.5">
       <c r="D42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:251" ht="12.75"/>
     <row r="44" spans="1:251" ht="13.5">
       <c r="A44" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -29208,7 +29209,7 @@
         </is>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46">
         <v>33</v>
@@ -29267,34 +29268,34 @@
         </is>
       </c>
       <c r="M1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W1" t="inlineStr">
         <is>
@@ -29302,24 +29303,24 @@
         </is>
       </c>
       <c r="X1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="13.5">
       <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
         <v>138</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>139</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>140</v>
-      </c>
-      <c r="E2" t="s">
-        <v>141</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -29327,16 +29328,16 @@
         </is>
       </c>
       <c r="G2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
         <v>138</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>139</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>140</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -29746,7 +29747,7 @@
     </row>
     <row r="12" spans="1:25" ht="13.5">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="42">
         <f>27-2</f>
@@ -29883,7 +29884,7 @@
     </row>
     <row r="19" spans="1:25" ht="13.5">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
@@ -29953,7 +29954,7 @@
     </row>
     <row r="22" spans="1:25" ht="13.5">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M22" s="46"/>
       <c r="N22" s="46"/>
@@ -29974,7 +29975,7 @@
     </row>
     <row r="24" spans="1:25" ht="13.5">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P24" s="44">
         <f>SUM(P3:P6)+P11+P12+P17+P19+P21+P22</f>
@@ -30077,7 +30078,7 @@
         </is>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
@@ -30102,7 +30103,7 @@
         </is>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -30122,7 +30123,7 @@
         </is>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -30147,7 +30148,7 @@
         </is>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="13.5">
@@ -30162,10 +30163,10 @@
         </is>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -30207,7 +30208,7 @@
   <sheetData>
     <row r="1" spans="1:249" customHeight="1" ht="15.75">
       <c r="A1" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
@@ -30708,16 +30709,16 @@
     <row r="3" spans="1:249" ht="13.5">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
         <v>113</v>
       </c>
-      <c r="C3" t="s">
-        <v>114</v>
-      </c>
       <c r="D3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
         <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>114</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -31471,46 +31472,46 @@
     </row>
     <row r="8" spans="1:249" ht="13.5">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="41">
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:249" ht="13.5">
       <c r="E9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:249" ht="13.5">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11">
         <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11">
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:249" ht="13.5">
       <c r="E12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:249" ht="13.5"/>
@@ -31773,19 +31774,19 @@
     </row>
     <row r="16" spans="1:249" ht="13.5">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16">
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:249" ht="13.5"/>
@@ -31799,13 +31800,13 @@
         <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19">
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:249" ht="13.5">
@@ -31817,7 +31818,7 @@
     </row>
     <row r="23" spans="1:249" ht="13.5">
       <c r="A23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -32072,41 +32073,41 @@
     </row>
     <row r="25" spans="1:249" ht="13.5">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25">
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25">
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:249" ht="13.5">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28">
         <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D28">
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:249" ht="13.5">
       <c r="C29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>